<commit_message>
Completed draft of velocity activity.
</commit_message>
<xml_diff>
--- a/spreadsheets/rates_of_change.xlsx
+++ b/spreadsheets/rates_of_change.xlsx
@@ -58,7 +58,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -75,6 +75,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFE0C2CD"/>
         <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFD7"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -112,7 +118,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -122,6 +128,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -154,7 +164,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFFFFFD7"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -699,10 +709,10 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="n">
+      <c r="A62" s="3" t="n">
         <v>60</v>
       </c>
-      <c r="B62" s="2" t="n">
+      <c r="B62" s="3" t="n">
         <v>858.834626701122</v>
       </c>
     </row>

</xml_diff>